<commit_message>
Map of USA with groups
</commit_message>
<xml_diff>
--- a/Excel/Indivisible_groups_by_county_type2.xlsx
+++ b/Excel/Indivisible_groups_by_county_type2.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perez_g\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perez_g\Desktop\Politics Data\Indivisble_ACP\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B2785D-FA7C-4C92-A8E7-A86F545A4459}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA671AAA-F9DF-4222-B08C-9AA27B80A146}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{204C4836-121A-49E0-852B-D8A77EF4F16B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Per Capita Chart" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$F$17</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Summary Sheet'!$B$1:$F$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -325,6 +326,967 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Indivisible</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Groups per 100,000 People</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Summary Sheet'!$C$3:$C$17</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>Exurbs</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Graying America</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>African American South</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Evangelical Hubs</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Working Class Country</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Military Posts</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Urban Suburbs</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Hispanic Centers</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Native American Lands</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Rural Middle America</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>College Towns</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>LDS Enclaves</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Aging Farmlands</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Big Cities</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Middle Suburbs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Summary Sheet'!$F$3:$F$17</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.1898523456441374</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4275465335917863</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.53972709821183562</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7700332892535583</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1453558217326125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0758376859146612</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5656073044476568</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.72890378237784592</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.97694889091877157</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5437400315669185</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.3083842643306443</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.19904186931024601</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.53738112681657213</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4792126004649502</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1336475941876252</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E781-45B8-B0E8-43E1E5DD4ACC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1729915695"/>
+        <c:axId val="1641926607"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1729915695"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1641926607"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1641926607"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1729915695"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{F8B20D13-F24A-4E9D-95AA-5505798C06EF}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="111" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8666892" cy="6281351"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8ABB348-3AC5-49F9-99EA-DBD5D4148C4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -630,7 +1592,7 @@
   <dimension ref="B1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
New data for 2016 by counties
</commit_message>
<xml_diff>
--- a/Excel/Indivisible_groups_by_county_type2.xlsx
+++ b/Excel/Indivisible_groups_by_county_type2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perez_g\Desktop\Politics Data\Indivisble_ACP\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A65BE43-3B21-4986-9470-7CCF95AD298E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8722F060-F40E-42B7-A315-EEB1C7C62273}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1935" yWindow="495" windowWidth="24270" windowHeight="13425" xr2:uid="{204C4836-121A-49E0-852B-D8A77EF4F16B}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Per Capita Chart" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Summary Sheet'!$B$1:$I$17</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Summary Sheet'!$B$1:$J$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Number of Indivisible Groups by American Communities Project County Classification</t>
   </si>
@@ -97,16 +97,19 @@
     <t>Population</t>
   </si>
   <si>
-    <t>GOP</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>GOP %</t>
   </si>
   <si>
     <t>Groups Per 100k</t>
+  </si>
+  <si>
+    <t>Votes Democrats</t>
+  </si>
+  <si>
+    <t>Votes GOP</t>
+  </si>
+  <si>
+    <t>Total Votes</t>
   </si>
 </sst>
 </file>
@@ -394,12 +397,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -408,6 +405,12 @@
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1695,10 +1698,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:I18"/>
+  <dimension ref="B1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,11 +1710,11 @@
     <col min="3" max="3" width="25.140625" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="7" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="7" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1722,8 +1725,9 @@
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
     </row>
-    <row r="2" spans="2:9" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="20" t="s">
         <v>1</v>
       </c>
@@ -1737,19 +1741,22 @@
         <v>19</v>
       </c>
       <c r="F2" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="I2" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="26" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="3" spans="2:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12">
         <v>1</v>
       </c>
@@ -1767,16 +1774,20 @@
         <v>1.1898523456441374</v>
       </c>
       <c r="G3" s="17">
-        <v>8944862</v>
+        <v>6226561</v>
       </c>
       <c r="H3" s="16">
-        <v>15864434</v>
-      </c>
-      <c r="I3" s="27">
-        <v>0.56383114999999995</v>
+        <v>9089568</v>
+      </c>
+      <c r="I3" s="16">
+        <v>16322055</v>
+      </c>
+      <c r="J3" s="25">
+        <f>H3/I3</f>
+        <v>0.55688870059560514</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="13">
         <v>2</v>
       </c>
@@ -1794,16 +1805,20 @@
         <v>2.4275465335917863</v>
       </c>
       <c r="G4" s="15">
-        <v>4352233</v>
+        <v>2770461</v>
       </c>
       <c r="H4" s="16">
-        <v>7366954</v>
-      </c>
-      <c r="I4" s="27">
-        <v>0.59077782000000001</v>
+        <v>4476309</v>
+      </c>
+      <c r="I4" s="16">
+        <v>7651492</v>
+      </c>
+      <c r="J4" s="25">
+        <f t="shared" ref="J4:J17" si="1">H4/I4</f>
+        <v>0.58502433250926744</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="13">
         <v>3</v>
       </c>
@@ -1821,16 +1836,20 @@
         <v>0.53972709821183562</v>
       </c>
       <c r="G5" s="15">
-        <v>3333140</v>
+        <v>3283025</v>
       </c>
       <c r="H5" s="16">
-        <v>6737378</v>
-      </c>
-      <c r="I5" s="27">
-        <v>0.49472361999999998</v>
+        <v>3356556</v>
+      </c>
+      <c r="I5" s="16">
+        <v>6842056</v>
+      </c>
+      <c r="J5" s="25">
+        <f t="shared" si="1"/>
+        <v>0.49057710138589922</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="13">
         <v>4</v>
       </c>
@@ -1848,16 +1867,20 @@
         <v>0.7700332892535583</v>
       </c>
       <c r="G6" s="15">
-        <v>3699581</v>
+        <v>1158545</v>
       </c>
       <c r="H6" s="16">
-        <v>5016888</v>
-      </c>
-      <c r="I6" s="27">
-        <v>0.73742547000000003</v>
+        <v>3717714</v>
+      </c>
+      <c r="I6" s="16">
+        <v>5061071</v>
+      </c>
+      <c r="J6" s="25">
+        <f t="shared" si="1"/>
+        <v>0.73457060768363058</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="13">
         <v>5</v>
       </c>
@@ -1875,16 +1898,20 @@
         <v>1.1453558217326125</v>
       </c>
       <c r="G7" s="15">
-        <v>2627426</v>
+        <v>919405</v>
       </c>
       <c r="H7" s="16">
-        <v>3684383</v>
-      </c>
-      <c r="I7" s="27">
-        <v>0.71312509999999996</v>
+        <v>2644426</v>
+      </c>
+      <c r="I7" s="16">
+        <v>3722982</v>
+      </c>
+      <c r="J7" s="25">
+        <f t="shared" si="1"/>
+        <v>0.71029782040310696</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="13">
         <v>6</v>
       </c>
@@ -1902,16 +1929,20 @@
         <v>1.0758376859146612</v>
       </c>
       <c r="G8" s="15">
-        <v>2218284</v>
+        <v>1558535</v>
       </c>
       <c r="H8" s="16">
-        <v>3947332</v>
-      </c>
-      <c r="I8" s="27">
-        <v>0.56197047</v>
+        <v>2263719</v>
+      </c>
+      <c r="I8" s="16">
+        <v>4062847</v>
+      </c>
+      <c r="J8" s="25">
+        <f t="shared" si="1"/>
+        <v>0.55717554709788486</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="13">
         <v>7</v>
       </c>
@@ -1929,16 +1960,20 @@
         <v>1.5656073044476568</v>
       </c>
       <c r="G9" s="15">
-        <v>11196148</v>
+        <v>17373073</v>
       </c>
       <c r="H9" s="16">
-        <v>29026350</v>
-      </c>
-      <c r="I9" s="27">
-        <v>0.38572359000000001</v>
+        <v>11616976</v>
+      </c>
+      <c r="I9" s="16">
+        <v>30585482</v>
+      </c>
+      <c r="J9" s="25">
+        <f t="shared" si="1"/>
+        <v>0.37981994202347374</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="13">
         <v>8</v>
       </c>
@@ -1956,16 +1991,20 @@
         <v>0.72890378237784592</v>
       </c>
       <c r="G10" s="15">
-        <v>1538688</v>
+        <v>1690947</v>
       </c>
       <c r="H10" s="16">
-        <v>3242687</v>
-      </c>
-      <c r="I10" s="27">
-        <v>0.47451018</v>
+        <v>1634342</v>
+      </c>
+      <c r="I10" s="16">
+        <v>3521813</v>
+      </c>
+      <c r="J10" s="25">
+        <f t="shared" si="1"/>
+        <v>0.46406268589502053</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="13">
         <v>9</v>
       </c>
@@ -1983,16 +2022,20 @@
         <v>0.97694889091877157</v>
       </c>
       <c r="G11" s="15">
-        <v>248144</v>
+        <v>110002</v>
       </c>
       <c r="H11" s="16">
-        <v>483409</v>
-      </c>
-      <c r="I11" s="27">
-        <v>0.51332102000000002</v>
+        <v>124074</v>
+      </c>
+      <c r="I11" s="16">
+        <v>254809</v>
+      </c>
+      <c r="J11" s="25">
+        <f t="shared" si="1"/>
+        <v>0.48692942556974045</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="13">
         <v>10</v>
       </c>
@@ -2010,16 +2053,20 @@
         <v>1.5437400315669185</v>
       </c>
       <c r="G12" s="15">
-        <v>6041521</v>
+        <v>3260468</v>
       </c>
       <c r="H12" s="16">
-        <v>9777145</v>
-      </c>
-      <c r="I12" s="27">
-        <v>0.61792281999999998</v>
+        <v>6115287</v>
+      </c>
+      <c r="I12" s="16">
+        <v>9993133</v>
+      </c>
+      <c r="J12" s="25">
+        <f t="shared" si="1"/>
+        <v>0.61194892532702205</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="13">
         <v>11</v>
       </c>
@@ -2037,16 +2084,20 @@
         <v>2.3083842643306443</v>
       </c>
       <c r="G13" s="15">
-        <v>3820668</v>
+        <v>4189499</v>
       </c>
       <c r="H13" s="16">
-        <v>8436420</v>
-      </c>
-      <c r="I13" s="27">
-        <v>0.45287788000000001</v>
+        <v>3896913</v>
+      </c>
+      <c r="I13" s="16">
+        <v>8725361</v>
+      </c>
+      <c r="J13" s="25">
+        <f t="shared" si="1"/>
+        <v>0.44661911409739952</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="13">
         <v>12</v>
       </c>
@@ -2064,16 +2115,20 @@
         <v>0.19904186931024601</v>
       </c>
       <c r="G14" s="15">
-        <v>546106</v>
+        <v>325646</v>
       </c>
       <c r="H14" s="16">
-        <v>1120519</v>
-      </c>
-      <c r="I14" s="27">
-        <v>0.48736879999999999</v>
+        <v>609026</v>
+      </c>
+      <c r="I14" s="16">
+        <v>1267503</v>
+      </c>
+      <c r="J14" s="25">
+        <f t="shared" si="1"/>
+        <v>0.4804927483406351</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="13">
         <v>13</v>
       </c>
@@ -2091,16 +2146,20 @@
         <v>0.53738112681657213</v>
       </c>
       <c r="G15" s="15">
-        <v>213059</v>
+        <v>57294</v>
       </c>
       <c r="H15" s="16">
-        <v>284742</v>
-      </c>
-      <c r="I15" s="27">
-        <v>0.74825280000000005</v>
+        <v>214344</v>
+      </c>
+      <c r="I15" s="16">
+        <v>288194</v>
+      </c>
+      <c r="J15" s="25">
+        <f t="shared" si="1"/>
+        <v>0.74374900240810005</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="13">
         <v>14</v>
       </c>
@@ -2118,16 +2177,20 @@
         <v>1.4792126004649502</v>
       </c>
       <c r="G16" s="15">
-        <v>8326247</v>
+        <v>19579545</v>
       </c>
       <c r="H16" s="16">
-        <v>27670334</v>
-      </c>
-      <c r="I16" s="27">
-        <v>0.30090879999999998</v>
+        <v>8877551</v>
+      </c>
+      <c r="I16" s="16">
+        <v>30088106</v>
+      </c>
+      <c r="J16" s="25">
+        <f t="shared" si="1"/>
+        <v>0.29505183875648405</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="14">
         <v>15</v>
       </c>
@@ -2145,21 +2208,25 @@
         <v>1.1336475941876252</v>
       </c>
       <c r="G17" s="18">
-        <v>4088908</v>
+        <v>3120882</v>
       </c>
       <c r="H17" s="19">
-        <v>7496298</v>
-      </c>
-      <c r="I17" s="28">
-        <v>0.54545697000000004</v>
+        <v>4153243</v>
+      </c>
+      <c r="I17" s="19">
+        <v>7654025</v>
+      </c>
+      <c r="J17" s="26">
+        <f t="shared" si="1"/>
+        <v>0.54262208445883053</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E18" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:F17">
     <cfRule type="colorScale" priority="4">
@@ -2171,7 +2238,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I17">
+  <conditionalFormatting sqref="J3:J17">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2184,6 +2251,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="88" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="78" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Charts for GOP share
</commit_message>
<xml_diff>
--- a/Excel/Indivisible_groups_by_county_type2.xlsx
+++ b/Excel/Indivisible_groups_by_county_type2.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perez_g\Desktop\Politics Data\Indivisble_ACP\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8722F060-F40E-42B7-A315-EEB1C7C62273}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E92884-08C5-4971-8FE1-C5846A7280D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1935" yWindow="495" windowWidth="24270" windowHeight="13425" xr2:uid="{204C4836-121A-49E0-852B-D8A77EF4F16B}"/>
+    <workbookView xWindow="2280" yWindow="840" windowWidth="24270" windowHeight="13425" xr2:uid="{204C4836-121A-49E0-852B-D8A77EF4F16B}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Sheet" sheetId="1" r:id="rId1"/>
-    <sheet name="Per Capita Chart" sheetId="2" r:id="rId2"/>
+    <sheet name="Per Capita Groups Chart" sheetId="2" r:id="rId2"/>
+    <sheet name="GOP Share Chart" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Summary Sheet'!$B$1:$J$17</definedName>
@@ -119,7 +120,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -368,9 +369,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -400,10 +398,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -411,6 +409,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -811,7 +812,420 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Trump</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Share of Total Votes by County Type, 2016</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF7C80"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Summary Sheet'!$C$3:$C$17</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>Exurbs</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Graying America</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>African American South</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Evangelical Hubs</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Working Class Country</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Military Posts</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Urban Suburbs</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Hispanic Centers</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Native American Lands</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Rural Middle America</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>College Towns</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>LDS Enclaves</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Aging Farmlands</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Big Cities</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Middle Suburbs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Summary Sheet'!$J$3:$J$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.55688870059560514</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.58502433250926744</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.49057710138589922</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.73457060768363058</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.71029782040310696</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55717554709788486</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.37981994202347374</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.46406268589502053</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.48692942556974045</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.61194892532702205</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.44661911409739952</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.4804927483406351</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.74374900240810005</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.29505183875648405</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.54262208445883053</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8197-4310-B52A-BCA3A8E3E631}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1436536144"/>
+        <c:axId val="1347298144"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1436536144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1347298144"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1347298144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1436536144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1354,8 +1768,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{F8B20D13-F24A-4E9D-95AA-5505798C06EF}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="89" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{1077D57B-BC9B-4C36-B48E-4DEC752E9C02}">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="89" workbookViewId="0" zoomToFit="1"/>
@@ -1376,6 +2304,39 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8ABB348-3AC5-49F9-99EA-DBD5D4148C4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8679522" cy="6303624"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41A4D781-0EB3-41D4-8D0D-93AA9A085CF7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1701,7 +2662,7 @@
   <dimension ref="B1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1715,49 +2676,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="2:10" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="23" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1773,22 +2734,22 @@
         <f t="shared" ref="F3:F16" si="0">(D3/E3)*100000</f>
         <v>1.1898523456441374</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="16">
         <v>6226561</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="15">
         <v>9089568</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="15">
         <v>16322055</v>
       </c>
-      <c r="J3" s="25">
+      <c r="J3" s="24">
         <f>H3/I3</f>
         <v>0.55688870059560514</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1804,22 +2765,22 @@
         <f t="shared" si="0"/>
         <v>2.4275465335917863</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="14">
         <v>2770461</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="15">
         <v>4476309</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="15">
         <v>7651492</v>
       </c>
-      <c r="J4" s="25">
+      <c r="J4" s="24">
         <f t="shared" ref="J4:J17" si="1">H4/I4</f>
         <v>0.58502433250926744</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="13">
+      <c r="B5" s="12">
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1835,22 +2796,22 @@
         <f t="shared" si="0"/>
         <v>0.53972709821183562</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="14">
         <v>3283025</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="15">
         <v>3356556</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="15">
         <v>6842056</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="24">
         <f t="shared" si="1"/>
         <v>0.49057710138589922</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="13">
+      <c r="B6" s="12">
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1866,22 +2827,22 @@
         <f t="shared" si="0"/>
         <v>0.7700332892535583</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="14">
         <v>1158545</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="15">
         <v>3717714</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="15">
         <v>5061071</v>
       </c>
-      <c r="J6" s="25">
+      <c r="J6" s="24">
         <f t="shared" si="1"/>
         <v>0.73457060768363058</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="13">
+      <c r="B7" s="12">
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1897,22 +2858,22 @@
         <f t="shared" si="0"/>
         <v>1.1453558217326125</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="14">
         <v>919405</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="15">
         <v>2644426</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="15">
         <v>3722982</v>
       </c>
-      <c r="J7" s="25">
+      <c r="J7" s="24">
         <f t="shared" si="1"/>
         <v>0.71029782040310696</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="13">
+      <c r="B8" s="12">
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1928,22 +2889,22 @@
         <f t="shared" si="0"/>
         <v>1.0758376859146612</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="14">
         <v>1558535</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="15">
         <v>2263719</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="15">
         <v>4062847</v>
       </c>
-      <c r="J8" s="25">
+      <c r="J8" s="24">
         <f t="shared" si="1"/>
         <v>0.55717554709788486</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="13">
+      <c r="B9" s="12">
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1959,22 +2920,22 @@
         <f t="shared" si="0"/>
         <v>1.5656073044476568</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="14">
         <v>17373073</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="15">
         <v>11616976</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9" s="15">
         <v>30585482</v>
       </c>
-      <c r="J9" s="25">
+      <c r="J9" s="24">
         <f t="shared" si="1"/>
         <v>0.37981994202347374</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="13">
+      <c r="B10" s="12">
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1990,22 +2951,22 @@
         <f t="shared" si="0"/>
         <v>0.72890378237784592</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="14">
         <v>1690947</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="15">
         <v>1634342</v>
       </c>
-      <c r="I10" s="16">
+      <c r="I10" s="15">
         <v>3521813</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J10" s="24">
         <f t="shared" si="1"/>
         <v>0.46406268589502053</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="13">
+      <c r="B11" s="12">
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -2021,22 +2982,22 @@
         <f t="shared" si="0"/>
         <v>0.97694889091877157</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="14">
         <v>110002</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="15">
         <v>124074</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="15">
         <v>254809</v>
       </c>
-      <c r="J11" s="25">
+      <c r="J11" s="24">
         <f t="shared" si="1"/>
         <v>0.48692942556974045</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="13">
+      <c r="B12" s="12">
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -2052,22 +3013,22 @@
         <f t="shared" si="0"/>
         <v>1.5437400315669185</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="14">
         <v>3260468</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="15">
         <v>6115287</v>
       </c>
-      <c r="I12" s="16">
+      <c r="I12" s="15">
         <v>9993133</v>
       </c>
-      <c r="J12" s="25">
+      <c r="J12" s="24">
         <f t="shared" si="1"/>
         <v>0.61194892532702205</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="13">
+      <c r="B13" s="12">
         <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -2083,22 +3044,22 @@
         <f t="shared" si="0"/>
         <v>2.3083842643306443</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="14">
         <v>4189499</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="15">
         <v>3896913</v>
       </c>
-      <c r="I13" s="16">
+      <c r="I13" s="15">
         <v>8725361</v>
       </c>
-      <c r="J13" s="25">
+      <c r="J13" s="24">
         <f t="shared" si="1"/>
         <v>0.44661911409739952</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="13">
+      <c r="B14" s="12">
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -2114,22 +3075,22 @@
         <f t="shared" si="0"/>
         <v>0.19904186931024601</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="14">
         <v>325646</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14" s="15">
         <v>609026</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14" s="15">
         <v>1267503</v>
       </c>
-      <c r="J14" s="25">
+      <c r="J14" s="24">
         <f t="shared" si="1"/>
         <v>0.4804927483406351</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="13">
+      <c r="B15" s="12">
         <v>13</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -2145,22 +3106,22 @@
         <f t="shared" si="0"/>
         <v>0.53738112681657213</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15" s="14">
         <v>57294</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="15">
         <v>214344</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I15" s="15">
         <v>288194</v>
       </c>
-      <c r="J15" s="25">
+      <c r="J15" s="24">
         <f t="shared" si="1"/>
         <v>0.74374900240810005</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="13">
+      <c r="B16" s="12">
         <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -2176,22 +3137,22 @@
         <f t="shared" si="0"/>
         <v>1.4792126004649502</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="14">
         <v>19579545</v>
       </c>
-      <c r="H16" s="16">
+      <c r="H16" s="15">
         <v>8877551</v>
       </c>
-      <c r="I16" s="16">
+      <c r="I16" s="15">
         <v>30088106</v>
       </c>
-      <c r="J16" s="25">
+      <c r="J16" s="24">
         <f t="shared" si="1"/>
         <v>0.29505183875648405</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="14">
+      <c r="B17" s="13">
         <v>15</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -2207,16 +3168,16 @@
         <f>(D17/E17)*100000</f>
         <v>1.1336475941876252</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="17">
         <v>3120882</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="18">
         <v>4153243</v>
       </c>
-      <c r="I17" s="19">
+      <c r="I17" s="18">
         <v>7654025</v>
       </c>
-      <c r="J17" s="26">
+      <c r="J17" s="25">
         <f t="shared" si="1"/>
         <v>0.54262208445883053</v>
       </c>

</xml_diff>

<commit_message>
Median edu by county type
</commit_message>
<xml_diff>
--- a/Excel/Indivisible_groups_by_county_type2.xlsx
+++ b/Excel/Indivisible_groups_by_county_type2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perez_g\Desktop\Politics Data\Indivisble_ACP\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E92884-08C5-4971-8FE1-C5846A7280D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B446368C-91F4-47B3-86FB-1B39A1E0C4CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="840" windowWidth="24270" windowHeight="13425" xr2:uid="{204C4836-121A-49E0-852B-D8A77EF4F16B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{204C4836-121A-49E0-852B-D8A77EF4F16B}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Sheet" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Number of Indivisible Groups by American Communities Project County Classification</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Total Votes</t>
+  </si>
+  <si>
+    <t>Median pct BA</t>
   </si>
 </sst>
 </file>
@@ -347,7 +350,7 @@
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -413,6 +416,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -423,6 +431,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF9966FF"/>
+      <color rgb="FF9933FF"/>
       <color rgb="FFFF7C80"/>
       <color rgb="FFFF5050"/>
     </mruColors>
@@ -2659,10 +2669,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:J18"/>
+  <dimension ref="B1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="B1" sqref="B1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2672,10 +2682,10 @@
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
     <col min="7" max="9" width="12.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="10" max="11" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
@@ -2687,8 +2697,9 @@
       <c r="H1" s="28"/>
       <c r="I1" s="28"/>
       <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
     </row>
-    <row r="2" spans="2:10" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
@@ -2716,8 +2727,11 @@
       <c r="J2" s="23" t="s">
         <v>20</v>
       </c>
+      <c r="K2" s="29" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="2:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11">
         <v>1</v>
       </c>
@@ -2747,8 +2761,11 @@
         <f>H3/I3</f>
         <v>0.55688870059560514</v>
       </c>
+      <c r="K3" s="30">
+        <v>0.28000000000000003</v>
+      </c>
     </row>
-    <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="12">
         <v>2</v>
       </c>
@@ -2778,8 +2795,11 @@
         <f t="shared" ref="J4:J17" si="1">H4/I4</f>
         <v>0.58502433250926744</v>
       </c>
+      <c r="K4" s="30">
+        <v>0.20100000000000001</v>
+      </c>
     </row>
-    <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="12">
         <v>3</v>
       </c>
@@ -2809,8 +2829,11 @@
         <f t="shared" si="1"/>
         <v>0.49057710138589922</v>
       </c>
+      <c r="K5" s="30">
+        <v>0.14399999999999999</v>
+      </c>
     </row>
-    <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="12">
         <v>4</v>
       </c>
@@ -2840,8 +2863,11 @@
         <f t="shared" si="1"/>
         <v>0.73457060768363058</v>
       </c>
+      <c r="K6" s="30">
+        <v>0.151</v>
+      </c>
     </row>
-    <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="12">
         <v>5</v>
       </c>
@@ -2871,8 +2897,11 @@
         <f t="shared" si="1"/>
         <v>0.71029782040310696</v>
       </c>
+      <c r="K7" s="30">
+        <v>0.14499999999999999</v>
+      </c>
     </row>
-    <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="12">
         <v>6</v>
       </c>
@@ -2902,8 +2931,11 @@
         <f t="shared" si="1"/>
         <v>0.55717554709788486</v>
       </c>
+      <c r="K8" s="30">
+        <v>0.24149999999999999</v>
+      </c>
     </row>
-    <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -2933,8 +2965,11 @@
         <f t="shared" si="1"/>
         <v>0.37981994202347374</v>
       </c>
+      <c r="K9" s="30">
+        <v>0.35699999999999998</v>
+      </c>
     </row>
-    <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="12">
         <v>8</v>
       </c>
@@ -2964,8 +2999,11 @@
         <f t="shared" si="1"/>
         <v>0.46406268589502053</v>
       </c>
+      <c r="K10" s="30">
+        <v>0.15</v>
+      </c>
     </row>
-    <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="12">
         <v>9</v>
       </c>
@@ -2995,8 +3033,11 @@
         <f t="shared" si="1"/>
         <v>0.48692942556974045</v>
       </c>
+      <c r="K11" s="30">
+        <v>0.1595</v>
+      </c>
     </row>
-    <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="12">
         <v>10</v>
       </c>
@@ -3026,8 +3067,11 @@
         <f t="shared" si="1"/>
         <v>0.61194892532702205</v>
       </c>
+      <c r="K12" s="30">
+        <v>0.19800000000000001</v>
+      </c>
     </row>
-    <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="12">
         <v>11</v>
       </c>
@@ -3057,8 +3101,11 @@
         <f t="shared" si="1"/>
         <v>0.44661911409739952</v>
       </c>
+      <c r="K13" s="30">
+        <v>0.33400000000000002</v>
+      </c>
     </row>
-    <row r="14" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -3088,8 +3135,11 @@
         <f t="shared" si="1"/>
         <v>0.4804927483406351</v>
       </c>
+      <c r="K14" s="30">
+        <v>0.21199999999999999</v>
+      </c>
     </row>
-    <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="12">
         <v>13</v>
       </c>
@@ -3119,8 +3169,11 @@
         <f t="shared" si="1"/>
         <v>0.74374900240810005</v>
       </c>
+      <c r="K15" s="30">
+        <v>0.20100000000000001</v>
+      </c>
     </row>
-    <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="12">
         <v>14</v>
       </c>
@@ -3150,8 +3203,11 @@
         <f t="shared" si="1"/>
         <v>0.29505183875648405</v>
       </c>
+      <c r="K16" s="30">
+        <v>0.32300000000000001</v>
+      </c>
     </row>
-    <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="13">
         <v>15</v>
       </c>
@@ -3181,16 +3237,19 @@
         <f t="shared" si="1"/>
         <v>0.54262208445883053</v>
       </c>
+      <c r="K17" s="31">
+        <v>0.251</v>
+      </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E18" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:F17">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3200,7 +3259,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J17">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="num" val="0.5"/>
@@ -3211,6 +3270,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF9966FF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="78" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Maps of national indivisible groups
</commit_message>
<xml_diff>
--- a/Excel/Indivisible_groups_by_county_type2.xlsx
+++ b/Excel/Indivisible_groups_by_county_type2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perez_g\Desktop\Politics Data\Indivisble_ACP\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B446368C-91F4-47B3-86FB-1B39A1E0C4CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDC206B-31BE-4DB7-9D38-5C94AC9121DF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{204C4836-121A-49E0-852B-D8A77EF4F16B}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="GOP Share Chart" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Summary Sheet'!$B$1:$J$17</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Summary Sheet'!$B$1:$K$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2672,7 +2672,7 @@
   <dimension ref="B1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K1"/>
+      <selection activeCell="B1" sqref="B1:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3281,6 +3281,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="78" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="70" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Per capita standard deviation calcs
</commit_message>
<xml_diff>
--- a/Excel/Indivisible_groups_by_county_type2.xlsx
+++ b/Excel/Indivisible_groups_by_county_type2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perez_g\Desktop\Politics Data\Indivisble_ACP\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9031DCD0-D25F-471D-BCCB-CC32E644CC17}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC642C5-CAE1-4039-BA53-0683C5C7B6C6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{204C4836-121A-49E0-852B-D8A77EF4F16B}"/>
   </bookViews>
@@ -417,9 +417,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -431,6 +428,9 @@
     </xf>
     <xf numFmtId="39" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2683,7 +2683,7 @@
   <dimension ref="B1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2698,19 +2698,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
     </row>
     <row r="2" spans="2:12" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="17" t="s">
@@ -2760,12 +2760,12 @@
       <c r="E3" s="6">
         <v>36391070</v>
       </c>
-      <c r="F3" s="30">
+      <c r="F3" s="29">
         <f t="shared" ref="F3:F16" si="0">(D3/E3)*100000</f>
         <v>1.1898523456441374</v>
       </c>
-      <c r="G3" s="28">
-        <v>2.9564805000000001</v>
+      <c r="G3" s="27">
+        <v>1.7623044999999999</v>
       </c>
       <c r="H3" s="14">
         <v>6226561</v>
@@ -2780,7 +2780,7 @@
         <f>I3/J3</f>
         <v>0.55688870059560514</v>
       </c>
-      <c r="L3" s="28">
+      <c r="L3" s="27">
         <v>0.28000000000000003</v>
       </c>
     </row>
@@ -2797,12 +2797,12 @@
       <c r="E4" s="6">
         <v>16765899</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F4" s="29">
         <f t="shared" si="0"/>
         <v>2.4275465335917863</v>
       </c>
-      <c r="G4" s="28">
-        <v>1.9369684</v>
+      <c r="G4" s="27">
+        <v>9.6566320000000001</v>
       </c>
       <c r="H4" s="12">
         <v>2770461</v>
@@ -2817,7 +2817,7 @@
         <f t="shared" ref="K4:K17" si="1">I4/J4</f>
         <v>0.58502433250926744</v>
       </c>
-      <c r="L4" s="28">
+      <c r="L4" s="27">
         <v>0.20100000000000001</v>
       </c>
     </row>
@@ -2834,12 +2834,12 @@
       <c r="E5" s="6">
         <v>16489815</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="29">
         <f t="shared" si="0"/>
         <v>0.53972709821183562</v>
       </c>
-      <c r="G5" s="28">
-        <v>0.74466288999999997</v>
+      <c r="G5" s="27">
+        <v>1.5693873</v>
       </c>
       <c r="H5" s="12">
         <v>3283025</v>
@@ -2854,7 +2854,7 @@
         <f t="shared" si="1"/>
         <v>0.49057710138589922</v>
       </c>
-      <c r="L5" s="28">
+      <c r="L5" s="27">
         <v>0.14399999999999999</v>
       </c>
     </row>
@@ -2871,12 +2871,12 @@
       <c r="E6" s="6">
         <v>12596858</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F6" s="29">
         <f t="shared" si="0"/>
         <v>0.7700332892535583</v>
       </c>
-      <c r="G6" s="28">
-        <v>0.54553026000000004</v>
+      <c r="G6" s="27">
+        <v>1.4682225</v>
       </c>
       <c r="H6" s="12">
         <v>1158545</v>
@@ -2891,7 +2891,7 @@
         <f t="shared" si="1"/>
         <v>0.73457060768363058</v>
       </c>
-      <c r="L6" s="28">
+      <c r="L6" s="27">
         <v>0.151</v>
       </c>
     </row>
@@ -2908,12 +2908,12 @@
       <c r="E7" s="6">
         <v>8556293</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="29">
         <f t="shared" si="0"/>
         <v>1.1453558217326125</v>
       </c>
-      <c r="G7" s="28">
-        <v>0.64239774000000005</v>
+      <c r="G7" s="27">
+        <v>2.6775264000000001</v>
       </c>
       <c r="H7" s="12">
         <v>919405</v>
@@ -2928,7 +2928,7 @@
         <f t="shared" si="1"/>
         <v>0.71029782040310696</v>
       </c>
-      <c r="L7" s="28">
+      <c r="L7" s="27">
         <v>0.14499999999999999</v>
       </c>
     </row>
@@ -2945,12 +2945,12 @@
       <c r="E8" s="6">
         <v>10596394</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="29">
         <f t="shared" si="0"/>
         <v>1.0758376859146612</v>
       </c>
-      <c r="G8" s="28">
-        <v>2.1425811000000001</v>
+      <c r="G8" s="27">
+        <v>1.8481508</v>
       </c>
       <c r="H8" s="12">
         <v>1558535</v>
@@ -2965,7 +2965,7 @@
         <f t="shared" si="1"/>
         <v>0.55717554709788486</v>
       </c>
-      <c r="L8" s="28">
+      <c r="L8" s="27">
         <v>0.24149999999999999</v>
       </c>
     </row>
@@ -2982,12 +2982,12 @@
       <c r="E9" s="6">
         <v>70707386</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9" s="29">
         <f t="shared" si="0"/>
         <v>1.5656073044476568</v>
       </c>
-      <c r="G9" s="28">
-        <v>9.8999758999999994</v>
+      <c r="G9" s="27">
+        <v>1.1985889000000001</v>
       </c>
       <c r="H9" s="12">
         <v>17373073</v>
@@ -3002,7 +3002,7 @@
         <f t="shared" si="1"/>
         <v>0.37981994202347374</v>
       </c>
-      <c r="L9" s="28">
+      <c r="L9" s="27">
         <v>0.35699999999999998</v>
       </c>
     </row>
@@ -3019,12 +3019,12 @@
       <c r="E10" s="6">
         <v>12484501</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="29">
         <f t="shared" si="0"/>
         <v>0.72890378237784592</v>
       </c>
-      <c r="G10" s="28">
-        <v>1.1447965</v>
+      <c r="G10" s="27">
+        <v>2.8235128999999999</v>
       </c>
       <c r="H10" s="12">
         <v>1690947</v>
@@ -3039,7 +3039,7 @@
         <f t="shared" si="1"/>
         <v>0.46406268589502053</v>
       </c>
-      <c r="L10" s="28">
+      <c r="L10" s="27">
         <v>0.15</v>
       </c>
     </row>
@@ -3056,12 +3056,12 @@
       <c r="E11" s="6">
         <v>818876</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F11" s="29">
         <f t="shared" si="0"/>
         <v>0.97694889091877157</v>
       </c>
-      <c r="G11" s="28">
-        <v>0.44172610000000001</v>
+      <c r="G11" s="27">
+        <v>2.0728118000000002</v>
       </c>
       <c r="H11" s="12">
         <v>110002</v>
@@ -3076,7 +3076,7 @@
         <f t="shared" si="1"/>
         <v>0.48692942556974045</v>
       </c>
-      <c r="L11" s="28">
+      <c r="L11" s="27">
         <v>0.1595</v>
       </c>
     </row>
@@ -3093,12 +3093,12 @@
       <c r="E12" s="6">
         <v>21441434</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="29">
         <f t="shared" si="0"/>
         <v>1.5437400315669185</v>
       </c>
-      <c r="G12" s="28">
-        <v>1.2090057000000001</v>
+      <c r="G12" s="27">
+        <v>2.8955213999999998</v>
       </c>
       <c r="H12" s="12">
         <v>3260468</v>
@@ -3113,7 +3113,7 @@
         <f t="shared" si="1"/>
         <v>0.61194892532702205</v>
       </c>
-      <c r="L12" s="28">
+      <c r="L12" s="27">
         <v>0.19800000000000001</v>
       </c>
     </row>
@@ -3130,12 +3130,12 @@
       <c r="E13" s="6">
         <v>19277553</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="29">
         <f t="shared" si="0"/>
         <v>2.3083842643306443</v>
       </c>
-      <c r="G13" s="28">
-        <v>4.3623345999999996</v>
+      <c r="G13" s="27">
+        <v>2.5529674</v>
       </c>
       <c r="H13" s="12">
         <v>4189499</v>
@@ -3150,7 +3150,7 @@
         <f t="shared" si="1"/>
         <v>0.44661911409739952</v>
       </c>
-      <c r="L13" s="28">
+      <c r="L13" s="27">
         <v>0.33400000000000002</v>
       </c>
     </row>
@@ -3167,12 +3167,12 @@
       <c r="E14" s="6">
         <v>3516848</v>
       </c>
-      <c r="F14" s="30">
+      <c r="F14" s="29">
         <f t="shared" si="0"/>
         <v>0.19904186931024601</v>
       </c>
-      <c r="G14" s="28">
-        <v>0.44172610000000001</v>
+      <c r="G14" s="27">
+        <v>0.83783985000000005</v>
       </c>
       <c r="H14" s="12">
         <v>325646</v>
@@ -3187,7 +3187,7 @@
         <f t="shared" si="1"/>
         <v>0.4804927483406351</v>
       </c>
-      <c r="L14" s="28">
+      <c r="L14" s="27">
         <v>0.21199999999999999</v>
       </c>
     </row>
@@ -3204,12 +3204,12 @@
       <c r="E15" s="6">
         <v>558263</v>
       </c>
-      <c r="F15" s="30">
+      <c r="F15" s="29">
         <f t="shared" si="0"/>
         <v>0.53738112681657213</v>
       </c>
-      <c r="G15" s="28">
-        <v>0.13564888999999999</v>
+      <c r="G15" s="27">
+        <v>3.1696260999999999</v>
       </c>
       <c r="H15" s="12">
         <v>57294</v>
@@ -3224,7 +3224,7 @@
         <f t="shared" si="1"/>
         <v>0.74374900240810005</v>
       </c>
-      <c r="L15" s="28">
+      <c r="L15" s="27">
         <v>0.20100000000000001</v>
       </c>
     </row>
@@ -3241,12 +3241,12 @@
       <c r="E16" s="6">
         <v>80448206</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="29">
         <f t="shared" si="0"/>
         <v>1.4792126004649502</v>
       </c>
-      <c r="G16" s="28">
-        <v>25.323604</v>
+      <c r="G16" s="27">
+        <v>1.3909813</v>
       </c>
       <c r="H16" s="12">
         <v>19579545</v>
@@ -3261,7 +3261,7 @@
         <f t="shared" si="1"/>
         <v>0.29505183875648405</v>
       </c>
-      <c r="L16" s="28">
+      <c r="L16" s="27">
         <v>0.32300000000000001</v>
       </c>
     </row>
@@ -3278,12 +3278,12 @@
       <c r="E17" s="7">
         <v>16495426</v>
       </c>
-      <c r="F17" s="31">
+      <c r="F17" s="30">
         <f>(D17/E17)*100000</f>
         <v>1.1336475941876252</v>
       </c>
-      <c r="G17" s="29">
-        <v>2.1497269999999999</v>
+      <c r="G17" s="28">
+        <v>0.91483930999999996</v>
       </c>
       <c r="H17" s="15">
         <v>3120882</v>
@@ -3298,7 +3298,7 @@
         <f t="shared" si="1"/>
         <v>0.54262208445883053</v>
       </c>
-      <c r="L17" s="29">
+      <c r="L17" s="28">
         <v>0.251</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New sheet with conditional formatting
</commit_message>
<xml_diff>
--- a/Excel/Indivisible_groups_by_county_type2.xlsx
+++ b/Excel/Indivisible_groups_by_county_type2.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perez_g\Desktop\Politics Data\Indivisble_ACP\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC642C5-CAE1-4039-BA53-0683C5C7B6C6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDBCB35-8A41-4E9B-9BBD-15C8905872AA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{204C4836-121A-49E0-852B-D8A77EF4F16B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary Sheet" sheetId="1" r:id="rId1"/>
-    <sheet name="Per Capita Groups Chart" sheetId="2" r:id="rId2"/>
-    <sheet name="GOP Share Chart" sheetId="3" r:id="rId3"/>
+    <sheet name="Small Summary" sheetId="4" r:id="rId1"/>
+    <sheet name="Summary Sheet" sheetId="1" r:id="rId2"/>
+    <sheet name="Per Capita Groups Chart" sheetId="2" r:id="rId3"/>
+    <sheet name="GOP Share Chart" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Summary Sheet'!$B$1:$K$17</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Small Summary'!$B$2:$G$18</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Summary Sheet'!$B$1:$L$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
   <si>
     <t>Number of Indivisible Groups by American Communities Project County Classification</t>
   </si>
@@ -117,6 +119,12 @@
   </si>
   <si>
     <t>StDev</t>
+  </si>
+  <si>
+    <t>Number of Indivisible Postings</t>
+  </si>
+  <si>
+    <t>Number of Indivisible Group Postings by American Communities Project County Classification</t>
   </si>
 </sst>
 </file>
@@ -353,7 +361,7 @@
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -429,8 +437,17 @@
     <xf numFmtId="39" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2296,7 +2313,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{F8B20D13-F24A-4E9D-95AA-5505798C06EF}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="89" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="111" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2307,7 +2324,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{1077D57B-BC9B-4C36-B48E-4DEC752E9C02}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="89" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="111" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2318,7 +2335,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8679522" cy="6303624"/>
+    <xdr:ext cx="8658311" cy="6281351"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2351,7 +2368,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8679522" cy="6303624"/>
+    <xdr:ext cx="8658311" cy="6281351"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2676,15 +2693,463 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{518D2AD3-BA13-420D-9286-F9C51453B19F}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:O19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="11" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+    </row>
+    <row r="3" spans="2:12" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2">
+        <v>433</v>
+      </c>
+      <c r="E4" s="6">
+        <v>36391000</v>
+      </c>
+      <c r="F4" s="29">
+        <f t="shared" ref="F4:F17" si="0">(D4/E4)*100000</f>
+        <v>1.1898546343876233</v>
+      </c>
+      <c r="G4" s="27">
+        <v>1.7623044999999999</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="32"/>
+    </row>
+    <row r="5" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="10">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>407</v>
+      </c>
+      <c r="E5" s="6">
+        <v>16766000</v>
+      </c>
+      <c r="F5" s="29">
+        <f t="shared" si="0"/>
+        <v>2.4275319098174881</v>
+      </c>
+      <c r="G5" s="27">
+        <v>9.6566320000000001</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="32"/>
+    </row>
+    <row r="6" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="10">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2">
+        <v>89</v>
+      </c>
+      <c r="E6" s="6">
+        <v>16490000</v>
+      </c>
+      <c r="F6" s="29">
+        <f t="shared" si="0"/>
+        <v>0.53972104305639779</v>
+      </c>
+      <c r="G6" s="27">
+        <v>1.5693873</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="32"/>
+    </row>
+    <row r="7" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="10">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2">
+        <v>97</v>
+      </c>
+      <c r="E7" s="6">
+        <v>12597000</v>
+      </c>
+      <c r="F7" s="29">
+        <f t="shared" si="0"/>
+        <v>0.77002460903389691</v>
+      </c>
+      <c r="G7" s="27">
+        <v>1.4682225</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="32"/>
+    </row>
+    <row r="8" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="10">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2">
+        <v>98</v>
+      </c>
+      <c r="E8" s="6">
+        <v>8556000</v>
+      </c>
+      <c r="F8" s="29">
+        <f t="shared" si="0"/>
+        <v>1.1453950444132772</v>
+      </c>
+      <c r="G8" s="27">
+        <v>2.6775264000000001</v>
+      </c>
+      <c r="H8" s="8"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="32"/>
+    </row>
+    <row r="9" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="10">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="2">
+        <v>114</v>
+      </c>
+      <c r="E9" s="6">
+        <v>10596000</v>
+      </c>
+      <c r="F9" s="29">
+        <f t="shared" si="0"/>
+        <v>1.0758776896942244</v>
+      </c>
+      <c r="G9" s="27">
+        <v>1.8481508</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="32"/>
+    </row>
+    <row r="10" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="10">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1107</v>
+      </c>
+      <c r="E10" s="6">
+        <v>70707000</v>
+      </c>
+      <c r="F10" s="29">
+        <f t="shared" si="0"/>
+        <v>1.5656158513301368</v>
+      </c>
+      <c r="G10" s="27">
+        <v>1.1985889000000001</v>
+      </c>
+      <c r="H10" s="8"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="32"/>
+    </row>
+    <row r="11" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="10">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="2">
+        <v>91</v>
+      </c>
+      <c r="E11" s="6">
+        <v>12485000</v>
+      </c>
+      <c r="F11" s="29">
+        <f t="shared" si="0"/>
+        <v>0.72887464957949544</v>
+      </c>
+      <c r="G11" s="27">
+        <v>2.8235128999999999</v>
+      </c>
+      <c r="H11" s="8"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="32"/>
+    </row>
+    <row r="12" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="10">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2">
+        <v>8</v>
+      </c>
+      <c r="E12" s="6">
+        <v>819000</v>
+      </c>
+      <c r="F12" s="29">
+        <f t="shared" si="0"/>
+        <v>0.97680097680097677</v>
+      </c>
+      <c r="G12" s="27">
+        <v>2.0728118000000002</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="32"/>
+    </row>
+    <row r="13" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="10">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="2">
+        <v>331</v>
+      </c>
+      <c r="E13" s="6">
+        <v>21441000</v>
+      </c>
+      <c r="F13" s="29">
+        <f t="shared" si="0"/>
+        <v>1.5437712793246585</v>
+      </c>
+      <c r="G13" s="27">
+        <v>2.8955213999999998</v>
+      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="32"/>
+    </row>
+    <row r="14" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="10">
+        <v>11</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="2">
+        <v>445</v>
+      </c>
+      <c r="E14" s="6">
+        <v>19278000</v>
+      </c>
+      <c r="F14" s="29">
+        <f t="shared" si="0"/>
+        <v>2.3083307397032886</v>
+      </c>
+      <c r="G14" s="27">
+        <v>2.5529674</v>
+      </c>
+      <c r="H14" s="8"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="32"/>
+    </row>
+    <row r="15" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="10">
+        <v>12</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="2">
+        <v>7</v>
+      </c>
+      <c r="E15" s="6">
+        <v>3517000</v>
+      </c>
+      <c r="F15" s="29">
+        <f t="shared" si="0"/>
+        <v>0.19903326698891102</v>
+      </c>
+      <c r="G15" s="27">
+        <v>0.83783985000000005</v>
+      </c>
+      <c r="H15" s="8"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="32"/>
+    </row>
+    <row r="16" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="10">
+        <v>13</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="2">
+        <v>3</v>
+      </c>
+      <c r="E16" s="6">
+        <v>558000</v>
+      </c>
+      <c r="F16" s="29">
+        <f t="shared" si="0"/>
+        <v>0.5376344086021505</v>
+      </c>
+      <c r="G16" s="27">
+        <v>3.1696260999999999</v>
+      </c>
+      <c r="H16" s="8"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="32"/>
+    </row>
+    <row r="17" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="10">
+        <v>14</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1190</v>
+      </c>
+      <c r="E17" s="6">
+        <v>80448000</v>
+      </c>
+      <c r="F17" s="29">
+        <f t="shared" si="0"/>
+        <v>1.4792163882259348</v>
+      </c>
+      <c r="G17" s="27">
+        <v>1.3909813</v>
+      </c>
+      <c r="H17" s="8"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="32"/>
+    </row>
+    <row r="18" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="11">
+        <v>15</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="5">
+        <v>187</v>
+      </c>
+      <c r="E18" s="7">
+        <v>16495000</v>
+      </c>
+      <c r="F18" s="30">
+        <f>(D18/E18)*100000</f>
+        <v>1.1336768717793271</v>
+      </c>
+      <c r="G18" s="28">
+        <v>0.91483930999999996</v>
+      </c>
+      <c r="H18" s="8"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="32"/>
+    </row>
+    <row r="19" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E19" s="8"/>
+      <c r="N19" s="33"/>
+      <c r="O19" s="32"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F4:F18">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="9" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4:G18">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF9966FF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F63CE5-12C5-41B6-AA8B-ACEF26962889}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:L18"/>
+  <dimension ref="B1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2697,22 +3162,22 @@
     <col min="10" max="11" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+    <row r="1" spans="2:15" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
     </row>
-    <row r="2" spans="2:12" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="17" t="s">
         <v>1</v>
       </c>
@@ -2747,7 +3212,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="9">
         <v>1</v>
       </c>
@@ -2783,8 +3248,10 @@
       <c r="L3" s="27">
         <v>0.28000000000000003</v>
       </c>
+      <c r="N3" s="31"/>
+      <c r="O3" s="32"/>
     </row>
-    <row r="4" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="10">
         <v>2</v>
       </c>
@@ -2820,8 +3287,10 @@
       <c r="L4" s="27">
         <v>0.20100000000000001</v>
       </c>
+      <c r="N4" s="33"/>
+      <c r="O4" s="32"/>
     </row>
-    <row r="5" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="10">
         <v>3</v>
       </c>
@@ -2857,8 +3326,10 @@
       <c r="L5" s="27">
         <v>0.14399999999999999</v>
       </c>
+      <c r="N5" s="33"/>
+      <c r="O5" s="32"/>
     </row>
-    <row r="6" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="10">
         <v>4</v>
       </c>
@@ -2894,8 +3365,10 @@
       <c r="L6" s="27">
         <v>0.151</v>
       </c>
+      <c r="N6" s="33"/>
+      <c r="O6" s="32"/>
     </row>
-    <row r="7" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="10">
         <v>5</v>
       </c>
@@ -2931,8 +3404,10 @@
       <c r="L7" s="27">
         <v>0.14499999999999999</v>
       </c>
+      <c r="N7" s="33"/>
+      <c r="O7" s="32"/>
     </row>
-    <row r="8" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <v>6</v>
       </c>
@@ -2968,8 +3443,10 @@
       <c r="L8" s="27">
         <v>0.24149999999999999</v>
       </c>
+      <c r="N8" s="33"/>
+      <c r="O8" s="32"/>
     </row>
-    <row r="9" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="10">
         <v>7</v>
       </c>
@@ -3005,8 +3482,10 @@
       <c r="L9" s="27">
         <v>0.35699999999999998</v>
       </c>
+      <c r="N9" s="33"/>
+      <c r="O9" s="32"/>
     </row>
-    <row r="10" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="10">
         <v>8</v>
       </c>
@@ -3042,8 +3521,10 @@
       <c r="L10" s="27">
         <v>0.15</v>
       </c>
+      <c r="N10" s="33"/>
+      <c r="O10" s="32"/>
     </row>
-    <row r="11" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>9</v>
       </c>
@@ -3079,8 +3560,10 @@
       <c r="L11" s="27">
         <v>0.1595</v>
       </c>
+      <c r="N11" s="33"/>
+      <c r="O11" s="32"/>
     </row>
-    <row r="12" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
         <v>10</v>
       </c>
@@ -3116,8 +3599,10 @@
       <c r="L12" s="27">
         <v>0.19800000000000001</v>
       </c>
+      <c r="N12" s="33"/>
+      <c r="O12" s="32"/>
     </row>
-    <row r="13" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
         <v>11</v>
       </c>
@@ -3153,8 +3638,10 @@
       <c r="L13" s="27">
         <v>0.33400000000000002</v>
       </c>
+      <c r="N13" s="33"/>
+      <c r="O13" s="32"/>
     </row>
-    <row r="14" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
         <v>12</v>
       </c>
@@ -3190,8 +3677,10 @@
       <c r="L14" s="27">
         <v>0.21199999999999999</v>
       </c>
+      <c r="N14" s="33"/>
+      <c r="O14" s="32"/>
     </row>
-    <row r="15" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
         <v>13</v>
       </c>
@@ -3227,8 +3716,10 @@
       <c r="L15" s="27">
         <v>0.20100000000000001</v>
       </c>
+      <c r="N15" s="33"/>
+      <c r="O15" s="32"/>
     </row>
-    <row r="16" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="10">
         <v>14</v>
       </c>
@@ -3264,8 +3755,10 @@
       <c r="L16" s="27">
         <v>0.32300000000000001</v>
       </c>
+      <c r="N16" s="33"/>
+      <c r="O16" s="32"/>
     </row>
-    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="11">
         <v>15</v>
       </c>
@@ -3301,9 +3794,13 @@
       <c r="L17" s="28">
         <v>0.251</v>
       </c>
+      <c r="N17" s="33"/>
+      <c r="O17" s="32"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E18" s="8"/>
+      <c r="N18" s="33"/>
+      <c r="O18" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3352,6 +3849,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="70" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="67" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>